<commit_message>
Updating to new version of validate without the regex bug.
</commit_message>
<xml_diff>
--- a/pyxform/tests/example_xls/xlsform_spec_test.xlsx
+++ b/pyxform/tests/example_xls/xlsform_spec_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="34" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="163">
   <si>
     <t>type</t>
   </si>
@@ -113,25 +113,31 @@
     <t>invalid_variable</t>
   </si>
   <si>
-    <t>Your name is ${my_name} ${my_name} ${my_name}</t>
+    <t>Your name is ${my_name}</t>
   </si>
   <si>
     <t>Try replacing my_name with a invalid variable</t>
   </si>
   <si>
-    <t>some_text</t>
-  </si>
-  <si>
-    <t>some text</t>
-  </si>
-  <si>
-    <t>a hint</t>
+    <t>address</t>
+  </si>
+  <si>
+    <t>Enter an address</t>
   </si>
   <si>
     <t>ni hao</t>
   </si>
   <si>
     <t>您好</t>
+  </si>
+  <si>
+    <t>email_note</t>
+  </si>
+  <si>
+    <t>You entered an email address</t>
+  </si>
+  <si>
+    <t>regex(${address}, '[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Za-z]{2,4}')</t>
   </si>
   <si>
     <t>number_label</t>
@@ -581,12 +587,18 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -604,767 +616,783 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T56"/>
+  <dimension ref="A1:T57"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F34" activeCellId="0" pane="topLeft" sqref="F34"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7490196078431"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7686274509804"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.8980392156863"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.3098039215686"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.3294117647059"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.8078431372549"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.4274509803922"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.53725490196078"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.5764705882353"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.53333333333333"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="51.9960784313725"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.0392156862745"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.7607843137255"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.5529411764706"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.3843137254902"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.0470588235294"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.721568627451"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.8823529411765"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="20.243137254902"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="21.0823529411765"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="12.878431372549"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.9647058823529"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.0313725490196"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="50.3960784313726"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="37.6862745098039"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="42.7607843137255"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="36.1686274509804"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.6627450980392"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.756862745098"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="7.6078431372549"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="52.521568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.1372549019608"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="23.9960784313725"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="12.678431372549"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.5137254901961"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.1725490196078"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="13.8549019607843"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="14.0274509803922"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="20.4509803921569"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="21.2980392156863"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="1" width="13.0039215686275"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="1">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="2">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="3">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="4">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="5">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="6">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="F6" s="0"/>
+      <c r="K6" s="0"/>
+      <c r="N6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="N6" s="0" t="s">
+      <c r="O6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="O6" s="2" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="7">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="7">
-      <c r="A7" s="0" t="s">
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="0"/>
+      <c r="K7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O7" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="8">
+      <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="0" t="n">
+      <c r="B8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="N7" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36.5" outlineLevel="0" r="8">
-      <c r="A8" s="0" t="s">
+      <c r="E8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" s="0"/>
+      <c r="N8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36.5" outlineLevel="0" r="9">
+      <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="N8" s="0" t="s">
+      <c r="B9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="O8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P8" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q8" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="R8" s="0" t="s">
+      <c r="P9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="S8" s="0" t="s">
+      <c r="Q9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="T8" s="0" t="s">
+      <c r="R9" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="9">
-      <c r="A9" s="0" t="s">
+      <c r="S9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="10">
+      <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="P9" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="10">
-      <c r="A10" s="0" t="s">
+      <c r="B10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="11">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="11">
-      <c r="A11" s="0" t="s">
+      <c r="B11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="12">
+      <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="23.75" outlineLevel="0" r="12">
-      <c r="A12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="D12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="23.75" outlineLevel="0" r="13">
+      <c r="A13" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="13">
-      <c r="A13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="14">
+      <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="14">
-      <c r="A14" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="F14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J14" s="0" t="n">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="15">
+      <c r="A15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="K14" s="4" t="b">
+      <c r="K15" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="15">
-      <c r="A15" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="1" t="s">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="16">
+      <c r="A16" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="16">
-      <c r="A16" s="0" t="s">
+      <c r="B16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="17">
+      <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="28.5" outlineLevel="0" r="17">
-      <c r="A17" s="0" t="s">
+      <c r="B17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="28.5" outlineLevel="0" r="18">
+      <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="H17" s="0" t="s">
+      <c r="B18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="19">
+      <c r="A19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="20">
+      <c r="A20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="21">
+      <c r="A21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="18">
-      <c r="A18" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="19">
-      <c r="A19" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="20">
-      <c r="A20" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="21">
-      <c r="A21" s="0" t="s">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="22">
+      <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="22">
-      <c r="A22" s="0" t="s">
+      <c r="B22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="23">
+      <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="H22" s="0" t="b">
+      <c r="B23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H23" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I22" s="0" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="23">
-      <c r="A23" s="0" t="s">
-        <v>76</v>
+      <c r="I23" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="24">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="25">
+      <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I24" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="25">
-      <c r="A25" s="0" t="s">
+      <c r="I25" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="26">
+      <c r="A26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="E25" s="0" t="s">
+      <c r="B26" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="26">
-      <c r="A26" s="0" t="s">
-        <v>76</v>
-      </c>
-    </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="27">
-      <c r="A27" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="I27" s="0" t="s">
+      <c r="A27" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="28">
+      <c r="A28" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="28">
-      <c r="A28" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="I28" s="0" t="s">
+      <c r="I28" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="29">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="D29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="30">
-      <c r="A30" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="B30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="31">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="1" t="s">
         <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="32">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" s="1" t="s">
         <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="33">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" s="1" t="s">
         <v>100</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="34">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D34" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="35">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="D35" s="1" t="s">
         <v>104</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="36">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="37">
+      <c r="A37" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="37">
-      <c r="A37" s="0" t="s">
+      <c r="B37" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="38">
+      <c r="A38" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="38">
-      <c r="A38" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D38" s="1" t="s">
         <v>108</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="39">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="40">
+      <c r="A40" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B39" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="40">
-      <c r="A40" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="M40" s="0" t="s">
+      <c r="D40" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="41">
+      <c r="A41" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="41">
-      <c r="A41" s="0" t="s">
+      <c r="B41" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="42">
+      <c r="A42" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B41" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="42">
-      <c r="A42" s="0" t="s">
+      <c r="B42" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B42" s="0" t="s">
-        <v>115</v>
+      <c r="D42" s="1" t="s">
+        <v>116</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="43">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="44">
+      <c r="A44" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B43" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="44">
-      <c r="A44" s="0" t="s">
+      <c r="B44" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B44" s="0" t="s">
-        <v>118</v>
+      <c r="D44" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="45">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="46">
+      <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B45" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="46">
-      <c r="A46" s="0" t="s">
+      <c r="B46" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B46" s="0" t="s">
-        <v>121</v>
+      <c r="D46" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="47">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="48">
+      <c r="A48" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B47" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="D47" s="0" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="48">
-      <c r="A48" s="0" t="s">
+      <c r="B48" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B48" s="0" t="s">
-        <v>124</v>
+      <c r="D48" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="49">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="50">
+      <c r="A50" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B49" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="50">
-      <c r="A50" s="0" t="s">
+      <c r="B50" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B50" s="0" t="s">
-        <v>127</v>
+      <c r="D50" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="51">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="52">
+      <c r="A52" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B51" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="52">
-      <c r="A52" s="0" t="s">
+      <c r="B52" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B52" s="0" t="s">
-        <v>130</v>
+      <c r="D52" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="53">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="54">
+      <c r="A54" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B53" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="54">
-      <c r="A54" s="0" t="s">
+      <c r="B54" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="55">
+      <c r="A55" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B54" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="55">
-      <c r="A55" s="0" t="s">
+      <c r="B55" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="56">
+      <c r="A56" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B55" s="0" t="b">
+      <c r="B56" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D55" s="0" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="56">
-      <c r="A56" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="B56" s="0" t="s">
+      <c r="D56" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="57">
+      <c r="A57" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1379,90 +1407,88 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="true" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomLeft" topLeftCell="A2" xSplit="0" ySplit="1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="F23" activeCellId="0" pane="bottomLeft" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3843137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5725490196078"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3960784313725"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="12.878431372549"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.5137254901961"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.7529411764706"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.5607843137255"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="13.0039215686275"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="1">
-      <c r="A1" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D1" s="0" t="s">
+      <c r="C1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="2">
-      <c r="A2" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>139</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="3">
-      <c r="A3" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>141</v>
+      <c r="A3" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="4">
-      <c r="A4" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="D4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>144</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="5">
-      <c r="A5" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>146</v>
+      <c r="A5" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1477,70 +1503,70 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E2" activeCellId="0" pane="topLeft" sqref="E2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.5686274509804"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2156862745098"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.3490196078431"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.4"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.2941176470588"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.3921568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.1529411764706"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.7333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.3490196078431"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="47.8156862745098"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.5725490196078"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.9803921568627"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="29.5843137254902"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="31.7019607843137"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="9.63137254901961"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="1">
-      <c r="A1" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>154</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="2">
-      <c r="A2" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="D2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F2" s="4" t="b">
+      <c r="B2" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G2" s="4" t="b">
+      <c r="G2" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H2" s="4" t="b">
+      <c r="H2" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1548,7 +1574,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1563,45 +1589,45 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="11.6666666666667"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="1">
-      <c r="A1" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="B1" s="0" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+      <c r="A1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="2">
-      <c r="A2" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="3">
-      <c r="A3" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="C1" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+      <c r="A2" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="B2" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+      <c r="A3" s="1" t="s">
         <v>160</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding autoplay attribute for media
</commit_message>
<xml_diff>
--- a/pyxform/tests/example_xls/xlsform_spec_test.xlsx
+++ b/pyxform/tests/example_xls/xlsform_spec_test.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="choices" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="settings" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="columns" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="survey" sheetId="1" r:id="rId1"/>
+    <sheet name="choices" sheetId="2" r:id="rId2"/>
+    <sheet name="settings" sheetId="3" r:id="rId3"/>
+    <sheet name="columns" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="164">
   <si>
     <t>type</t>
   </si>
@@ -507,40 +506,25 @@
   </si>
   <si>
     <t>buffalo</t>
+  </si>
+  <si>
+    <t>autoplay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-  </numFmts>
-  <fonts count="5">
+  <fonts count="2">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
       <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
       <name val="WenQuanYi Micro Hei"/>
       <family val="2"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -552,7 +536,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -560,93 +544,345 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:T57"/>
+  <dimension ref="A1:AMK57"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.9647058823529"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.0313725490196"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="50.3960784313726"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="37.6862745098039"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="42.7607843137255"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="36.1686274509804"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.6627450980392"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.61176470588235"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.756862745098"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="7.6078431372549"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="52.521568627451"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.1372549019608"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="23.9960784313725"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="12.678431372549"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.5137254901961"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.1725490196078"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="13.8549019607843"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="14.0274509803922"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="20.4509803921569"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="21.2980392156863"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="1" width="13.0039215686275"/>
+    <col min="1" max="1" width="21" style="1"/>
+    <col min="2" max="2" width="26" style="1"/>
+    <col min="3" max="3" width="50.42578125" style="1"/>
+    <col min="4" max="4" width="37.7109375" style="1"/>
+    <col min="5" max="5" width="42.7109375" style="1"/>
+    <col min="6" max="6" width="36.140625" style="1"/>
+    <col min="7" max="7" width="24.7109375" style="1"/>
+    <col min="8" max="8" width="8.5703125" style="1"/>
+    <col min="9" max="9" width="18.7109375" style="1"/>
+    <col min="10" max="10" width="7.5703125" style="1"/>
+    <col min="11" max="11" width="52.5703125" style="1"/>
+    <col min="12" max="12" width="10.140625" style="1"/>
+    <col min="13" max="13" width="24" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1"/>
+    <col min="15" max="15" width="13.5703125" style="1"/>
+    <col min="16" max="16" width="12.140625" style="1"/>
+    <col min="17" max="17" width="13.85546875" style="1"/>
+    <col min="18" max="18" width="14" style="1"/>
+    <col min="19" max="19" width="20.42578125" style="1"/>
+    <col min="20" max="20" width="21.28515625" style="1"/>
+    <col min="21" max="1025" width="13" style="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="1">
+    <row r="1" spans="1:21" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -707,8 +943,11 @@
       <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="2">
+      <c r="U1" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="16.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -719,7 +958,7 @@
         <v>22</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="3">
+    <row r="3" spans="1:21" ht="16.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -730,7 +969,7 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="4">
+    <row r="4" spans="1:21" ht="16.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -741,7 +980,7 @@
         <v>28</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="5">
+    <row r="5" spans="1:21" ht="16.5" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
@@ -755,7 +994,7 @@
         <v>32</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="6">
+    <row r="6" spans="1:21" ht="16.5" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -765,8 +1004,8 @@
       <c r="D6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="0"/>
-      <c r="K6" s="0"/>
+      <c r="F6"/>
+      <c r="K6"/>
       <c r="N6" s="1" t="s">
         <v>35</v>
       </c>
@@ -774,7 +1013,7 @@
         <v>36</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="7">
+    <row r="7" spans="1:21" ht="16.5" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -784,26 +1023,26 @@
       <c r="D7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="0"/>
+      <c r="F7"/>
       <c r="K7" s="2" t="s">
         <v>39</v>
       </c>
       <c r="O7" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="8">
+    <row r="8" spans="1:21" ht="16.5" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K8" s="0"/>
+      <c r="K8"/>
       <c r="N8" s="1" t="s">
         <v>42</v>
       </c>
@@ -811,7 +1050,7 @@
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36.5" outlineLevel="0" r="9">
+    <row r="9" spans="1:21" ht="36.6" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -845,8 +1084,11 @@
       <c r="T9" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="10">
+      <c r="U9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="16.5" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
@@ -857,7 +1099,7 @@
         <v>45</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="11">
+    <row r="11" spans="1:21" ht="16.5" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -871,7 +1113,7 @@
         <v>52</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="12">
+    <row r="12" spans="1:21" ht="16.5" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -885,7 +1127,7 @@
         <v>54</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="23.75" outlineLevel="0" r="13">
+    <row r="13" spans="1:21" ht="23.85" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>55</v>
       </c>
@@ -896,7 +1138,7 @@
         <v>57</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="14">
+    <row r="14" spans="1:21" ht="16.5" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
@@ -910,7 +1152,7 @@
         <v>61</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="15">
+    <row r="15" spans="1:21" ht="16.5" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>55</v>
       </c>
@@ -920,15 +1162,15 @@
       <c r="D15" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J15" s="1" t="n">
+      <c r="J15" s="1">
         <v>3</v>
       </c>
       <c r="K15" s="1" t="b">
-        <f aca="false">FALSE()</f>
+        <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="16">
+    <row r="16" spans="1:21" ht="16.5" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>64</v>
       </c>
@@ -942,7 +1184,7 @@
         <v>65</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="17">
+    <row r="17" spans="1:9" ht="16.5" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -953,7 +1195,7 @@
         <v>68</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="28.5" outlineLevel="0" r="18">
+    <row r="18" spans="1:9" ht="28.5" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -967,7 +1209,7 @@
         <v>70</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="19">
+    <row r="19" spans="1:9" ht="16.5" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>71</v>
       </c>
@@ -990,7 +1232,7 @@
         <v>77</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="20">
+    <row r="20" spans="1:9" ht="16.5" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>78</v>
       </c>
@@ -998,7 +1240,7 @@
         <v>79</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="21">
+    <row r="21" spans="1:9" ht="16.5" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1012,7 +1254,7 @@
         <v>68</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="22">
+    <row r="22" spans="1:9" ht="16.5" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1026,7 +1268,7 @@
         <v>83</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="23">
+    <row r="23" spans="1:9" ht="16.5" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -1037,19 +1279,19 @@
         <v>84</v>
       </c>
       <c r="H23" s="1" t="b">
-        <f aca="false">TRUE()</f>
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="24">
+    <row r="24" spans="1:9" ht="16.5" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="25">
+    <row r="25" spans="1:9" ht="16.5" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1060,7 +1302,7 @@
         <v>86</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="26">
+    <row r="26" spans="1:9" ht="16.5" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>20</v>
       </c>
@@ -1074,12 +1316,12 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="27">
+    <row r="27" spans="1:9" ht="16.5" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="28">
+    <row r="28" spans="1:9" ht="16.5" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>89</v>
       </c>
@@ -1093,7 +1335,7 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="29">
+    <row r="29" spans="1:9" ht="16.5" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>89</v>
       </c>
@@ -1107,12 +1349,12 @@
         <v>93</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="30">
+    <row r="30" spans="1:9" ht="16.5" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="31">
+    <row r="31" spans="1:9" ht="16.5" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>95</v>
       </c>
@@ -1123,7 +1365,7 @@
         <v>96</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="32">
+    <row r="32" spans="1:9" ht="16.5" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>97</v>
       </c>
@@ -1134,7 +1376,7 @@
         <v>98</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="33">
+    <row r="33" spans="1:13" ht="16.5" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>99</v>
       </c>
@@ -1145,7 +1387,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="34">
+    <row r="34" spans="1:13" ht="16.5" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>101</v>
       </c>
@@ -1156,7 +1398,7 @@
         <v>102</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="35">
+    <row r="35" spans="1:13" ht="16.5" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>103</v>
       </c>
@@ -1167,7 +1409,7 @@
         <v>104</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="36">
+    <row r="36" spans="1:13" ht="16.5" customHeight="1">
       <c r="A36" s="1" t="s">
         <v>105</v>
       </c>
@@ -1178,7 +1420,7 @@
         <v>106</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="37">
+    <row r="37" spans="1:13" ht="16.5" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>15</v>
       </c>
@@ -1189,7 +1431,7 @@
         <v>107</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="38">
+    <row r="38" spans="1:13" ht="16.5" customHeight="1">
       <c r="A38" s="1" t="s">
         <v>16</v>
       </c>
@@ -1200,7 +1442,7 @@
         <v>108</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="39">
+    <row r="39" spans="1:13" ht="16.5" customHeight="1">
       <c r="A39" s="1" t="s">
         <v>109</v>
       </c>
@@ -1211,7 +1453,7 @@
         <v>110</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="40">
+    <row r="40" spans="1:13" ht="16.5" customHeight="1">
       <c r="A40" s="1" t="s">
         <v>29</v>
       </c>
@@ -1222,7 +1464,7 @@
         <v>111</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="41">
+    <row r="41" spans="1:13" ht="16.5" customHeight="1">
       <c r="A41" s="1" t="s">
         <v>112</v>
       </c>
@@ -1233,7 +1475,7 @@
         <v>114</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="42">
+    <row r="42" spans="1:13" ht="16.5" customHeight="1">
       <c r="A42" s="1" t="s">
         <v>29</v>
       </c>
@@ -1244,7 +1486,7 @@
         <v>116</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="43">
+    <row r="43" spans="1:13" ht="16.5" customHeight="1">
       <c r="A43" s="1" t="s">
         <v>117</v>
       </c>
@@ -1252,7 +1494,7 @@
         <v>117</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="44">
+    <row r="44" spans="1:13" ht="16.5" customHeight="1">
       <c r="A44" s="1" t="s">
         <v>29</v>
       </c>
@@ -1263,7 +1505,7 @@
         <v>119</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="45">
+    <row r="45" spans="1:13" ht="16.5" customHeight="1">
       <c r="A45" s="1" t="s">
         <v>120</v>
       </c>
@@ -1271,7 +1513,7 @@
         <v>120</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="46">
+    <row r="46" spans="1:13" ht="16.5" customHeight="1">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
@@ -1282,7 +1524,7 @@
         <v>122</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="47">
+    <row r="47" spans="1:13" ht="16.5" customHeight="1">
       <c r="A47" s="1" t="s">
         <v>123</v>
       </c>
@@ -1290,7 +1532,7 @@
         <v>123</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="48">
+    <row r="48" spans="1:13" ht="16.5" customHeight="1">
       <c r="A48" s="1" t="s">
         <v>29</v>
       </c>
@@ -1301,7 +1543,7 @@
         <v>125</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="49">
+    <row r="49" spans="1:4" ht="16.5" customHeight="1">
       <c r="A49" s="1" t="s">
         <v>126</v>
       </c>
@@ -1309,7 +1551,7 @@
         <v>126</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="50">
+    <row r="50" spans="1:4" ht="16.5" customHeight="1">
       <c r="A50" s="1" t="s">
         <v>29</v>
       </c>
@@ -1320,7 +1562,7 @@
         <v>128</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="51">
+    <row r="51" spans="1:4" ht="16.5" customHeight="1">
       <c r="A51" s="1" t="s">
         <v>129</v>
       </c>
@@ -1328,7 +1570,7 @@
         <v>129</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="52">
+    <row r="52" spans="1:4" ht="16.5" customHeight="1">
       <c r="A52" s="1" t="s">
         <v>29</v>
       </c>
@@ -1339,7 +1581,7 @@
         <v>131</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="53">
+    <row r="53" spans="1:4" ht="16.5" customHeight="1">
       <c r="A53" s="1" t="s">
         <v>132</v>
       </c>
@@ -1347,7 +1589,7 @@
         <v>132</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="54">
+    <row r="54" spans="1:4" ht="16.5" customHeight="1">
       <c r="A54" s="1" t="s">
         <v>29</v>
       </c>
@@ -1358,7 +1600,7 @@
         <v>134</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="55">
+    <row r="55" spans="1:4" ht="16.5" customHeight="1">
       <c r="A55" s="1" t="s">
         <v>26</v>
       </c>
@@ -1369,19 +1611,19 @@
         <v>136</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="56">
+    <row r="56" spans="1:4" ht="16.5" customHeight="1">
       <c r="A56" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B56" s="1" t="b">
-        <f aca="false">FALSE()</f>
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="57">
+    <row r="57" spans="1:4" ht="16.5" customHeight="1">
       <c r="A57" s="1" t="s">
         <v>78</v>
       </c>
@@ -1390,35 +1632,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:AMK5"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.5137254901961"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.7529411764706"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.5607843137255"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="13.0039215686275"/>
+    <col min="1" max="1" width="13.5703125" style="1"/>
+    <col min="2" max="2" width="17.7109375" style="1"/>
+    <col min="3" max="3" width="16.5703125" style="1"/>
+    <col min="4" max="1025" width="13" style="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>138</v>
       </c>
@@ -1435,7 +1668,7 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>139</v>
       </c>
@@ -1449,7 +1682,7 @@
         <v>141</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="3">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>139</v>
       </c>
@@ -1463,7 +1696,7 @@
         <v>143</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="4">
+    <row r="4" spans="1:5" ht="12.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>144</v>
       </c>
@@ -1474,7 +1707,7 @@
         <v>146</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="5">
+    <row r="5" spans="1:5" ht="12.75" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>144</v>
       </c>
@@ -1486,40 +1719,31 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:AMK2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.1529411764706"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.7333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.3490196078431"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="47.8156862745098"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.5725490196078"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.9803921568627"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="29.5843137254902"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="31.7019607843137"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="9.63137254901961"/>
+    <col min="1" max="1" width="23.140625" style="1"/>
+    <col min="2" max="2" width="16.7109375" style="1"/>
+    <col min="3" max="3" width="13.28515625" style="1"/>
+    <col min="4" max="4" width="47.85546875" style="1"/>
+    <col min="5" max="5" width="17.5703125" style="1"/>
+    <col min="6" max="6" width="18" style="1"/>
+    <col min="7" max="7" width="29.5703125" style="1"/>
+    <col min="8" max="8" width="31.7109375" style="1"/>
+    <col min="9" max="1025" width="9.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>149</v>
       </c>
@@ -1545,7 +1769,7 @@
         <v>156</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>157</v>
       </c>
@@ -1559,45 +1783,36 @@
         <v>159</v>
       </c>
       <c r="F2" s="1" t="b">
-        <f aca="false">FALSE()</f>
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="G2" s="1" t="b">
-        <f aca="false">FALSE()</f>
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H2" s="1" t="b">
-        <f aca="false">TRUE()</f>
+        <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:AMK3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="11.6666666666667"/>
+    <col min="1" max="1025" width="11.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" spans="1:3" ht="12.75">
       <c r="A1" s="1" t="s">
         <v>138</v>
       </c>
@@ -1608,7 +1823,7 @@
         <v>83</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+    <row r="2" spans="1:3" ht="12.75">
       <c r="A2" s="1" t="s">
         <v>160</v>
       </c>
@@ -1619,7 +1834,7 @@
         <v>161</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+    <row r="3" spans="1:3" ht="12.75">
       <c r="A3" s="1" t="s">
         <v>160</v>
       </c>
@@ -1631,10 +1846,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Fixing orx:meta element bug and adding new features for upcoming collect release.
</commit_message>
<xml_diff>
--- a/pyxform/tests/example_xls/xlsform_spec_test.xlsx
+++ b/pyxform/tests/example_xls/xlsform_spec_test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
@@ -12,12 +12,12 @@
     <sheet name="settings" sheetId="3" r:id="rId3"/>
     <sheet name="columns" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="179">
   <si>
     <t>type</t>
   </si>
@@ -509,13 +509,58 @@
   </si>
   <si>
     <t>autoplay</t>
+  </si>
+  <si>
+    <t>buttonText</t>
+  </si>
+  <si>
+    <t>noAppErrorString</t>
+  </si>
+  <si>
+    <t>requiredMsg</t>
+  </si>
+  <si>
+    <t>launch</t>
+  </si>
+  <si>
+    <t>ex:org.thirdparty.app.ActivityName</t>
+  </si>
+  <si>
+    <t>This launches a fictional application to get an integer result.</t>
+  </si>
+  <si>
+    <t>Sorry, app does not exist.</t>
+  </si>
+  <si>
+    <t>Launch Fictional app</t>
+  </si>
+  <si>
+    <t>Custom required message.</t>
+  </si>
+  <si>
+    <t>instanceName</t>
+  </si>
+  <si>
+    <t>${my_name}</t>
+  </si>
+  <si>
+    <t>uri:deviceid</t>
+  </si>
+  <si>
+    <t>uri_deviceid</t>
+  </si>
+  <si>
+    <t>deviceid_test_output: ${uri_deviceid}</t>
+  </si>
+  <si>
+    <t>uri_deviceid_test_output</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -524,6 +569,12 @@
     <font>
       <sz val="10"/>
       <name val="WenQuanYi Micro Hei"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -549,7 +600,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -557,12 +608,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -641,6 +698,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -675,6 +733,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -850,14 +909,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AMK57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AML60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="21" style="1"/>
     <col min="2" max="2" width="26" style="1"/>
@@ -866,23 +925,27 @@
     <col min="5" max="5" width="42.7109375" style="1"/>
     <col min="6" max="6" width="36.140625" style="1"/>
     <col min="7" max="7" width="24.7109375" style="1"/>
-    <col min="8" max="8" width="8.5703125" style="1"/>
-    <col min="9" max="9" width="18.7109375" style="1"/>
-    <col min="10" max="10" width="7.5703125" style="1"/>
-    <col min="11" max="11" width="52.5703125" style="1"/>
-    <col min="12" max="12" width="10.140625" style="1"/>
-    <col min="13" max="13" width="24" style="1"/>
-    <col min="14" max="14" width="12.7109375" style="1"/>
-    <col min="15" max="15" width="13.5703125" style="1"/>
-    <col min="16" max="16" width="12.140625" style="1"/>
-    <col min="17" max="17" width="13.85546875" style="1"/>
-    <col min="18" max="18" width="14" style="1"/>
-    <col min="19" max="19" width="20.42578125" style="1"/>
-    <col min="20" max="20" width="21.28515625" style="1"/>
-    <col min="21" max="1025" width="13" style="1"/>
+    <col min="8" max="8" width="21.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" style="1"/>
+    <col min="10" max="10" width="18.7109375" style="1"/>
+    <col min="11" max="11" width="7.5703125" style="1"/>
+    <col min="12" max="12" width="52.5703125" style="1"/>
+    <col min="13" max="13" width="10.140625" style="1"/>
+    <col min="14" max="14" width="24" style="1"/>
+    <col min="15" max="15" width="12.7109375" style="1"/>
+    <col min="16" max="16" width="13.5703125" style="1"/>
+    <col min="17" max="17" width="12.140625" style="1"/>
+    <col min="18" max="18" width="13.85546875" style="1"/>
+    <col min="19" max="19" width="14" style="1"/>
+    <col min="20" max="20" width="20.42578125" style="1"/>
+    <col min="21" max="21" width="21.28515625" style="1"/>
+    <col min="22" max="22" width="13" style="1"/>
+    <col min="23" max="23" width="19.7109375" style="1" customWidth="1"/>
+    <col min="24" max="24" width="16.7109375" style="1" customWidth="1"/>
+    <col min="25" max="1026" width="13" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="16.5" customHeight="1">
+    <row r="1" spans="1:25" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -904,50 +967,60 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" ht="16.5" customHeight="1">
+      <c r="W1" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y1" s="5"/>
+    </row>
+    <row r="2" spans="1:25" ht="16.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -958,18 +1031,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="16.5" customHeight="1">
+    <row r="3" spans="1:25" ht="16.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="16.5" customHeight="1">
+    <row r="4" spans="1:25" ht="16.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -980,7 +1053,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="16.5" customHeight="1">
+    <row r="5" spans="1:25" ht="16.5" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
@@ -994,7 +1067,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="16.5" customHeight="1">
+    <row r="6" spans="1:25" ht="16.5" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -1005,15 +1078,15 @@
         <v>34</v>
       </c>
       <c r="F6"/>
-      <c r="K6"/>
-      <c r="N6" s="1" t="s">
+      <c r="L6"/>
+      <c r="O6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="16.5" customHeight="1">
+    <row r="7" spans="1:25" ht="16.5" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -1024,12 +1097,12 @@
         <v>38</v>
       </c>
       <c r="F7"/>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="O7" s="3"/>
-    </row>
-    <row r="8" spans="1:21" ht="16.5" customHeight="1">
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:25" ht="16.5" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -1042,15 +1115,15 @@
       <c r="E8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K8"/>
-      <c r="N8" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="L8"/>
       <c r="O8" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" ht="36.6" customHeight="1">
+      <c r="P8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="36.6" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -1063,43 +1136,43 @@
       <c r="E9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="P9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="S9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="S9" s="1" t="s">
+      <c r="T9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="U9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="U9" s="1" t="s">
+      <c r="V9" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="16.5" customHeight="1">
+    <row r="10" spans="1:25" ht="16.5" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="Q10" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="16.5" customHeight="1">
+    <row r="11" spans="1:25" ht="16.5" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1109,11 +1182,11 @@
       <c r="D11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="16.5" customHeight="1">
+    <row r="12" spans="1:25" ht="16.5" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -1123,11 +1196,11 @@
       <c r="D12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="23.85" customHeight="1">
+    <row r="13" spans="1:25" ht="23.85" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>55</v>
       </c>
@@ -1138,7 +1211,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="16.5" customHeight="1">
+    <row r="14" spans="1:25" ht="16.5" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
@@ -1152,7 +1225,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="16.5" customHeight="1">
+    <row r="15" spans="1:25" ht="16.5" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>55</v>
       </c>
@@ -1162,15 +1235,15 @@
       <c r="D15" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J15" s="1">
+      <c r="K15" s="1">
         <v>3</v>
       </c>
-      <c r="K15" s="1" t="b">
+      <c r="L15" s="1" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="16.5" customHeight="1">
+    <row r="16" spans="1:25" ht="16.5" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>64</v>
       </c>
@@ -1184,18 +1257,18 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="16.5" customHeight="1">
+    <row r="17" spans="1:10" ht="16.5" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="28.5" customHeight="1">
+    <row r="18" spans="1:10" ht="28.5" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -1206,10 +1279,13 @@
         <v>69</v>
       </c>
       <c r="H18" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="16.5" customHeight="1">
+    <row r="19" spans="1:10" ht="16.5" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>71</v>
       </c>
@@ -1225,14 +1301,14 @@
       <c r="G19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="16.5" customHeight="1">
+    <row r="20" spans="1:10" ht="16.5" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>78</v>
       </c>
@@ -1240,7 +1316,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="16.5" customHeight="1">
+    <row r="21" spans="1:10" ht="16.5" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1250,11 +1326,11 @@
       <c r="D21" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="16.5" customHeight="1">
+    <row r="22" spans="1:10" ht="16.5" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1264,11 +1340,11 @@
       <c r="D22" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="16.5" customHeight="1">
+    <row r="23" spans="1:10" ht="16.5" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -1278,31 +1354,31 @@
       <c r="D23" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H23" s="1" t="b">
+      <c r="I23" s="1" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="16.5" customHeight="1">
+    <row r="24" spans="1:10" ht="16.5" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="16.5" customHeight="1">
+    <row r="25" spans="1:10" ht="16.5" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="16.5" customHeight="1">
+    <row r="26" spans="1:10" ht="16.5" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>20</v>
       </c>
@@ -1316,12 +1392,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="16.5" customHeight="1">
+    <row r="27" spans="1:10" ht="16.5" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="16.5" customHeight="1">
+    <row r="28" spans="1:10" ht="16.5" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>89</v>
       </c>
@@ -1331,11 +1407,11 @@
       <c r="D28" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="16.5" customHeight="1">
+    <row r="29" spans="1:10" ht="16.5" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>89</v>
       </c>
@@ -1345,16 +1421,16 @@
       <c r="D29" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="J29" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="16.5" customHeight="1">
+    <row r="30" spans="1:10" ht="16.5" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="16.5" customHeight="1">
+    <row r="31" spans="1:10" ht="16.5" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>95</v>
       </c>
@@ -1365,7 +1441,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="16.5" customHeight="1">
+    <row r="32" spans="1:10" ht="16.5" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>97</v>
       </c>
@@ -1376,7 +1452,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="16.5" customHeight="1">
+    <row r="33" spans="1:14" ht="16.5" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>99</v>
       </c>
@@ -1387,7 +1463,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="16.5" customHeight="1">
+    <row r="34" spans="1:14" ht="16.5" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>101</v>
       </c>
@@ -1398,7 +1474,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="16.5" customHeight="1">
+    <row r="35" spans="1:14" ht="16.5" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>103</v>
       </c>
@@ -1409,7 +1485,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="16.5" customHeight="1">
+    <row r="36" spans="1:14" ht="16.5" customHeight="1">
       <c r="A36" s="1" t="s">
         <v>105</v>
       </c>
@@ -1420,7 +1496,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="16.5" customHeight="1">
+    <row r="37" spans="1:14" ht="16.5" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>15</v>
       </c>
@@ -1431,7 +1507,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="16.5" customHeight="1">
+    <row r="38" spans="1:14" ht="16.5" customHeight="1">
       <c r="A38" s="1" t="s">
         <v>16</v>
       </c>
@@ -1442,7 +1518,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="16.5" customHeight="1">
+    <row r="39" spans="1:14" ht="16.5" customHeight="1">
       <c r="A39" s="1" t="s">
         <v>109</v>
       </c>
@@ -1453,7 +1529,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="16.5" customHeight="1">
+    <row r="40" spans="1:14" ht="16.5" customHeight="1">
       <c r="A40" s="1" t="s">
         <v>29</v>
       </c>
@@ -1464,18 +1540,18 @@
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="16.5" customHeight="1">
+    <row r="41" spans="1:14" ht="16.5" customHeight="1">
       <c r="A41" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="M41" s="1" t="s">
+      <c r="N41" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="16.5" customHeight="1">
+    <row r="42" spans="1:14" ht="16.5" customHeight="1">
       <c r="A42" s="1" t="s">
         <v>29</v>
       </c>
@@ -1486,7 +1562,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="16.5" customHeight="1">
+    <row r="43" spans="1:14" ht="16.5" customHeight="1">
       <c r="A43" s="1" t="s">
         <v>117</v>
       </c>
@@ -1494,7 +1570,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="16.5" customHeight="1">
+    <row r="44" spans="1:14" ht="16.5" customHeight="1">
       <c r="A44" s="1" t="s">
         <v>29</v>
       </c>
@@ -1505,7 +1581,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="16.5" customHeight="1">
+    <row r="45" spans="1:14" ht="16.5" customHeight="1">
       <c r="A45" s="1" t="s">
         <v>120</v>
       </c>
@@ -1513,7 +1589,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="16.5" customHeight="1">
+    <row r="46" spans="1:14" ht="16.5" customHeight="1">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
@@ -1524,7 +1600,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="16.5" customHeight="1">
+    <row r="47" spans="1:14" ht="16.5" customHeight="1">
       <c r="A47" s="1" t="s">
         <v>123</v>
       </c>
@@ -1532,7 +1608,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="16.5" customHeight="1">
+    <row r="48" spans="1:14" ht="16.5" customHeight="1">
       <c r="A48" s="1" t="s">
         <v>29</v>
       </c>
@@ -1543,7 +1619,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="16.5" customHeight="1">
+    <row r="49" spans="1:24" ht="16.5" customHeight="1">
       <c r="A49" s="1" t="s">
         <v>126</v>
       </c>
@@ -1551,7 +1627,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="16.5" customHeight="1">
+    <row r="50" spans="1:24" ht="16.5" customHeight="1">
       <c r="A50" s="1" t="s">
         <v>29</v>
       </c>
@@ -1562,88 +1638,127 @@
         <v>128</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="16.5" customHeight="1">
+    <row r="51" spans="1:24" s="1" customFormat="1" ht="16.5" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>129</v>
+        <v>175</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="16.5" customHeight="1">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" s="1" customFormat="1" ht="16.5" customHeight="1">
       <c r="A52" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>130</v>
+        <v>178</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="16.5" customHeight="1">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" ht="16.5" customHeight="1">
       <c r="A53" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="16.5" customHeight="1">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" ht="16.5" customHeight="1">
       <c r="A54" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" ht="16.5" customHeight="1">
+      <c r="A55" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" ht="16.5" customHeight="1">
+      <c r="A56" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A55" s="1" t="s">
+    <row r="57" spans="1:24" ht="16.5" customHeight="1">
+      <c r="A57" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A56" s="1" t="s">
+    <row r="58" spans="1:24" ht="16.5" customHeight="1">
+      <c r="A58" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B56" s="1" t="b">
+      <c r="B58" s="1" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A57" s="1" t="s">
+    <row r="59" spans="1:24" ht="16.5" customHeight="1">
+      <c r="A59" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24">
+      <c r="A60" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="W60" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="X60" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="2400" verticalDpi="2400" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="13.5703125" style="1"/>
     <col min="2" max="2" width="17.7109375" style="1"/>
@@ -1725,12 +1840,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="23.140625" style="1"/>
     <col min="2" max="2" width="16.7109375" style="1"/>
@@ -1740,10 +1857,11 @@
     <col min="6" max="6" width="18" style="1"/>
     <col min="7" max="7" width="29.5703125" style="1"/>
     <col min="8" max="8" width="31.7109375" style="1"/>
-    <col min="9" max="1025" width="9.5703125" style="1"/>
+    <col min="9" max="9" width="14" style="1" customWidth="1"/>
+    <col min="10" max="1025" width="9.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>149</v>
       </c>
@@ -1768,8 +1886,11 @@
       <c r="H1" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1">
+      <c r="I1" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>157</v>
       </c>
@@ -1793,6 +1914,9 @@
       <c r="H2" s="1" t="b">
         <f>TRUE()</f>
         <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1802,17 +1926,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1025" width="11.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="12.75">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>138</v>
       </c>
@@ -1823,7 +1947,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="12.75">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>160</v>
       </c>
@@ -1834,7 +1958,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="12.75">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>160</v>
       </c>

</xml_diff>

<commit_message>
padding xpaths + generating repeat_count nodes + lowercasing column headers
</commit_message>
<xml_diff>
--- a/pyxform/tests/example_xls/xlsform_spec_test.xlsx
+++ b/pyxform/tests/example_xls/xlsform_spec_test.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="178">
   <si>
     <t>type</t>
   </si>
@@ -37,9 +37,6 @@
     <t>constraint</t>
   </si>
   <si>
-    <t>constraint_message</t>
-  </si>
-  <si>
     <t>required</t>
   </si>
   <si>
@@ -205,21 +202,12 @@
     <t>. &lt;= ${a_integer}</t>
   </si>
   <si>
-    <t>num_repeat_times</t>
-  </si>
-  <si>
-    <t>no label</t>
-  </si>
-  <si>
     <t>begin repeat</t>
   </si>
   <si>
     <t>repeat_test</t>
   </si>
   <si>
-    <t>${num_repeat_times}</t>
-  </si>
-  <si>
     <t>group_test</t>
   </si>
   <si>
@@ -244,9 +232,6 @@
     <t>not(selected(., 'yes') and selected (., 'no'))</t>
   </si>
   <si>
-    <t>you can't select yes and no</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -538,9 +523,6 @@
     <t>Custom required message.</t>
   </si>
   <si>
-    <t>instanceName</t>
-  </si>
-  <si>
     <t>${my_name}</t>
   </si>
   <si>
@@ -554,6 +536,21 @@
   </si>
   <si>
     <t>uri_deviceid_test_output</t>
+  </si>
+  <si>
+    <t>instance_name</t>
+  </si>
+  <si>
+    <t>Sorry ${my_name}, you can't select yes and no.</t>
+  </si>
+  <si>
+    <t>constraint_message::english</t>
+  </si>
+  <si>
+    <t>constraint_message::chinese</t>
+  </si>
+  <si>
+    <t>對不起 ${my_name}，你可以不選擇“是”和“否”。</t>
   </si>
 </sst>
 </file>
@@ -910,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AML60"/>
+  <dimension ref="A1:AMM59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -924,28 +921,28 @@
     <col min="4" max="4" width="37.7109375" style="1"/>
     <col min="5" max="5" width="42.7109375" style="1"/>
     <col min="6" max="6" width="36.140625" style="1"/>
-    <col min="7" max="7" width="24.7109375" style="1"/>
-    <col min="8" max="8" width="21.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" style="1"/>
-    <col min="10" max="10" width="18.7109375" style="1"/>
-    <col min="11" max="11" width="7.5703125" style="1"/>
-    <col min="12" max="12" width="52.5703125" style="1"/>
-    <col min="13" max="13" width="10.140625" style="1"/>
-    <col min="14" max="14" width="24" style="1"/>
-    <col min="15" max="15" width="12.7109375" style="1"/>
-    <col min="16" max="16" width="13.5703125" style="1"/>
-    <col min="17" max="17" width="12.140625" style="1"/>
-    <col min="18" max="18" width="13.85546875" style="1"/>
-    <col min="19" max="19" width="14" style="1"/>
-    <col min="20" max="20" width="20.42578125" style="1"/>
-    <col min="21" max="21" width="21.28515625" style="1"/>
-    <col min="22" max="22" width="13" style="1"/>
-    <col min="23" max="23" width="19.7109375" style="1" customWidth="1"/>
-    <col min="24" max="24" width="16.7109375" style="1" customWidth="1"/>
-    <col min="25" max="1026" width="13" style="1"/>
+    <col min="7" max="8" width="41.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" style="1"/>
+    <col min="11" max="11" width="18.7109375" style="1"/>
+    <col min="12" max="12" width="7.5703125" style="1"/>
+    <col min="13" max="13" width="52.5703125" style="1"/>
+    <col min="14" max="14" width="10.140625" style="1"/>
+    <col min="15" max="15" width="24" style="1"/>
+    <col min="16" max="16" width="12.7109375" style="1"/>
+    <col min="17" max="17" width="13.5703125" style="1"/>
+    <col min="18" max="18" width="12.140625" style="1"/>
+    <col min="19" max="19" width="13.85546875" style="1"/>
+    <col min="20" max="20" width="14" style="1"/>
+    <col min="21" max="21" width="20.42578125" style="1"/>
+    <col min="22" max="22" width="21.28515625" style="1"/>
+    <col min="23" max="23" width="13" style="1"/>
+    <col min="24" max="24" width="19.7109375" style="1" customWidth="1"/>
+    <col min="25" max="25" width="16.7109375" style="1" customWidth="1"/>
+    <col min="26" max="1027" width="13" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="16.5" customHeight="1">
+    <row r="1" spans="1:26" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -965,785 +962,773 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="Z1" s="5"/>
+    </row>
+    <row r="2" spans="1:26" ht="16.5" customHeight="1">
+      <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="Y1" s="5"/>
-    </row>
-    <row r="2" spans="1:25" ht="16.5" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:26" ht="16.5" customHeight="1">
+      <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" ht="16.5" customHeight="1">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:26" ht="16.5" customHeight="1">
+      <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" ht="16.5" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:26" ht="16.5" customHeight="1">
+      <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" ht="16.5" customHeight="1">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:26" ht="16.5" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" ht="16.5" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6"/>
+      <c r="M6"/>
+      <c r="P6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F6"/>
-      <c r="L6"/>
-      <c r="O6" s="1" t="s">
+      <c r="Q6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="P6" s="3" t="s">
+    </row>
+    <row r="7" spans="1:26" ht="16.5" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" ht="16.5" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7"/>
+      <c r="M7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F7"/>
-      <c r="L7" s="2" t="s">
+      <c r="Q7" s="3"/>
+    </row>
+    <row r="8" spans="1:26" ht="16.5" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="1:25" ht="16.5" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8"/>
+      <c r="P8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L8"/>
-      <c r="O8" s="1" t="s">
+      <c r="Q8" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="36.6" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" ht="36.6" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="E9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="P9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="R9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q9" s="1" t="s">
+      <c r="S9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="T9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="S9" s="1" t="s">
+      <c r="U9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="V9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="U9" s="1" t="s">
+      <c r="W9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="16.5" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="V9" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" ht="16.5" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="R10" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="16.5" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q10" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="16.5" customHeight="1">
-      <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="D11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J11" s="1" t="s">
+    </row>
+    <row r="12" spans="1:26" ht="16.5" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" ht="16.5" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:26" ht="23.85" customHeight="1">
+      <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" ht="23.85" customHeight="1">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="1" t="s">
+    </row>
+    <row r="14" spans="1:26" ht="16.5" customHeight="1">
+      <c r="A14" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" ht="16.5" customHeight="1">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="1" t="s">
+    </row>
+    <row r="15" spans="1:26" ht="16.5" customHeight="1">
+      <c r="A15" s="1" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" ht="16.5" customHeight="1">
-      <c r="A15" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C15" s="2">
+        <v>2</v>
+      </c>
       <c r="D15" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="16.5" customHeight="1">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K15" s="1">
-        <v>3</v>
-      </c>
-      <c r="L15" s="1" t="b">
+      <c r="K16" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="28.5" customHeight="1">
+      <c r="A17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J22" s="1" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A23" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A26" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A28" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A29" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A30" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A32" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A33" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A34" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A38" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A39" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A40" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A41" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A43" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A44" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A45" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A46" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A47" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A48" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" ht="16.5" customHeight="1">
+      <c r="A49" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" s="1" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A50" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" s="1" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A51" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" ht="16.5" customHeight="1">
+      <c r="A52" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25" ht="16.5" customHeight="1">
+      <c r="A53" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" ht="16.5" customHeight="1">
+      <c r="A54" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25" ht="16.5" customHeight="1">
+      <c r="A55" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25" ht="16.5" customHeight="1">
+      <c r="A56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25" ht="16.5" customHeight="1">
+      <c r="A57" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57" s="1" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" ht="16.5" customHeight="1">
-      <c r="A16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A17" s="1" t="s">
+      <c r="D57" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25" ht="16.5" customHeight="1">
+      <c r="A58" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A19" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A20" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A21" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="I23" s="1" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A24" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A27" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A28" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A29" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A30" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A31" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A32" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" ht="16.5" customHeight="1">
-      <c r="A33" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" ht="16.5" customHeight="1">
-      <c r="A34" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" ht="16.5" customHeight="1">
-      <c r="A35" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" ht="16.5" customHeight="1">
-      <c r="A36" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" ht="16.5" customHeight="1">
-      <c r="A37" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" ht="16.5" customHeight="1">
-      <c r="A38" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" ht="16.5" customHeight="1">
-      <c r="A39" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" ht="16.5" customHeight="1">
-      <c r="A40" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" ht="16.5" customHeight="1">
-      <c r="A41" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N41" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" ht="16.5" customHeight="1">
-      <c r="A42" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" ht="16.5" customHeight="1">
-      <c r="A43" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" ht="16.5" customHeight="1">
-      <c r="A44" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" ht="16.5" customHeight="1">
-      <c r="A45" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" ht="16.5" customHeight="1">
-      <c r="A46" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" ht="16.5" customHeight="1">
-      <c r="A47" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" ht="16.5" customHeight="1">
-      <c r="A48" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24" ht="16.5" customHeight="1">
-      <c r="A49" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="50" spans="1:24" ht="16.5" customHeight="1">
-      <c r="A50" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="51" spans="1:24" s="1" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A51" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="52" spans="1:24" s="1" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A52" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="53" spans="1:24" ht="16.5" customHeight="1">
-      <c r="A53" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="54" spans="1:24" ht="16.5" customHeight="1">
-      <c r="A54" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="55" spans="1:24" ht="16.5" customHeight="1">
-      <c r="A55" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="56" spans="1:24" ht="16.5" customHeight="1">
-      <c r="A56" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="57" spans="1:24" ht="16.5" customHeight="1">
-      <c r="A57" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="58" spans="1:24" ht="16.5" customHeight="1">
-      <c r="A58" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B58" s="1" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="59" spans="1:24" ht="16.5" customHeight="1">
+    </row>
+    <row r="59" spans="1:25">
       <c r="A59" s="1" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="60" spans="1:24">
-      <c r="A60" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J60" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="W60" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="X60" s="1" t="s">
-        <v>170</v>
+        <v>162</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="X59" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="Y59" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1768,69 +1753,69 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1844,7 +1829,7 @@
   <dimension ref="A1:AMK2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1863,28 +1848,28 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>173</v>
@@ -1892,16 +1877,16 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F2" s="1" t="b">
         <f>FALSE()</f>
@@ -1916,7 +1901,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -1938,35 +1923,35 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding support for rows column
</commit_message>
<xml_diff>
--- a/pyxform/tests/example_xls/xlsform_spec_test.xlsx
+++ b/pyxform/tests/example_xls/xlsform_spec_test.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="179">
   <si>
     <t>type</t>
   </si>
@@ -551,6 +551,9 @@
   </si>
   <si>
     <t>對不起 ${my_name}，你可以不選擇“是”和“否”。</t>
+  </si>
+  <si>
+    <t>rows</t>
   </si>
 </sst>
 </file>
@@ -907,42 +910,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMM59"/>
+  <dimension ref="A1:AMN59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="21" style="1"/>
     <col min="2" max="2" width="26" style="1"/>
-    <col min="3" max="3" width="50.42578125" style="1"/>
-    <col min="4" max="4" width="37.7109375" style="1"/>
-    <col min="5" max="5" width="42.7109375" style="1"/>
-    <col min="6" max="6" width="36.140625" style="1"/>
-    <col min="7" max="8" width="41.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" style="1"/>
-    <col min="11" max="11" width="18.7109375" style="1"/>
-    <col min="12" max="12" width="7.5703125" style="1"/>
-    <col min="13" max="13" width="52.5703125" style="1"/>
-    <col min="14" max="14" width="10.140625" style="1"/>
-    <col min="15" max="15" width="24" style="1"/>
-    <col min="16" max="16" width="12.7109375" style="1"/>
-    <col min="17" max="17" width="13.5703125" style="1"/>
-    <col min="18" max="18" width="12.140625" style="1"/>
-    <col min="19" max="19" width="13.85546875" style="1"/>
-    <col min="20" max="20" width="14" style="1"/>
-    <col min="21" max="21" width="20.42578125" style="1"/>
-    <col min="22" max="22" width="21.28515625" style="1"/>
-    <col min="23" max="23" width="13" style="1"/>
-    <col min="24" max="24" width="19.7109375" style="1" customWidth="1"/>
-    <col min="25" max="25" width="16.7109375" style="1" customWidth="1"/>
-    <col min="26" max="1027" width="13" style="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="50.42578125" style="1"/>
+    <col min="5" max="5" width="37.7109375" style="1"/>
+    <col min="6" max="6" width="42.7109375" style="1"/>
+    <col min="7" max="7" width="36.140625" style="1"/>
+    <col min="8" max="9" width="41.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="1"/>
+    <col min="12" max="12" width="18.7109375" style="1"/>
+    <col min="13" max="13" width="7.5703125" style="1"/>
+    <col min="14" max="14" width="52.5703125" style="1"/>
+    <col min="15" max="15" width="10.140625" style="1"/>
+    <col min="16" max="16" width="24" style="1"/>
+    <col min="17" max="17" width="12.7109375" style="1"/>
+    <col min="18" max="18" width="13.5703125" style="1"/>
+    <col min="19" max="19" width="12.140625" style="1"/>
+    <col min="20" max="20" width="13.85546875" style="1"/>
+    <col min="21" max="21" width="14" style="1"/>
+    <col min="22" max="22" width="20.42578125" style="1"/>
+    <col min="23" max="23" width="21.28515625" style="1"/>
+    <col min="24" max="24" width="13" style="1"/>
+    <col min="25" max="25" width="19.7109375" style="1" customWidth="1"/>
+    <col min="26" max="26" width="16.7109375" style="1" customWidth="1"/>
+    <col min="27" max="1028" width="13" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="16.5" customHeight="1">
+    <row r="1" spans="1:27" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -950,350 +954,356 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="Z1" s="5"/>
-    </row>
-    <row r="2" spans="1:26" ht="16.5" customHeight="1">
+      <c r="AA1" s="5"/>
+    </row>
+    <row r="2" spans="1:27" ht="16.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="16.5" customHeight="1">
+    <row r="3" spans="1:27" ht="16.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="16.5" customHeight="1">
+    <row r="4" spans="1:27" ht="16.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="1">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="16.5" customHeight="1">
+    <row r="5" spans="1:27" ht="16.5" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="16.5" customHeight="1">
+    <row r="6" spans="1:27" ht="16.5" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F6"/>
-      <c r="M6"/>
-      <c r="P6" s="1" t="s">
+      <c r="G6"/>
+      <c r="N6"/>
+      <c r="Q6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="R6" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="16.5" customHeight="1">
+    <row r="7" spans="1:27" ht="16.5" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F7"/>
-      <c r="M7" s="2" t="s">
+      <c r="G7"/>
+      <c r="N7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="Q7" s="3"/>
-    </row>
-    <row r="8" spans="1:26" ht="16.5" customHeight="1">
+      <c r="R7" s="3"/>
+    </row>
+    <row r="8" spans="1:27" ht="16.5" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>1</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M8"/>
-      <c r="P8" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="N8"/>
       <c r="Q8" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" ht="36.6" customHeight="1">
+      <c r="R8" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="36.6" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Q9" s="3" t="s">
+      <c r="R9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="S9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S9" s="1" t="s">
+      <c r="T9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="U9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U9" s="1" t="s">
+      <c r="V9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="V9" s="1" t="s">
+      <c r="W9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="W9" s="1" t="s">
+      <c r="X9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="16.5" customHeight="1">
+    <row r="10" spans="1:27" ht="16.5" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="S10" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="16.5" customHeight="1">
+    <row r="11" spans="1:27" ht="16.5" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="16.5" customHeight="1">
+    <row r="12" spans="1:27" ht="16.5" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="23.85" customHeight="1">
+    <row r="13" spans="1:27" ht="23.85" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="16.5" customHeight="1">
+    <row r="14" spans="1:27" ht="16.5" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="16.5" customHeight="1">
+    <row r="15" spans="1:27" ht="16.5" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="2">
+      <c r="D15" s="2">
         <v>2</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="16.5" customHeight="1">
+    <row r="16" spans="1:27" ht="16.5" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="28.5" customHeight="1">
+    <row r="17" spans="1:12" ht="28.5" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="16.5" customHeight="1">
+    <row r="18" spans="1:12" ht="16.5" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="16.5" customHeight="1">
+    <row r="19" spans="1:12" ht="16.5" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>73</v>
       </c>
@@ -1301,253 +1311,254 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="16.5" customHeight="1">
+    <row r="20" spans="1:12" ht="16.5" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="16.5" customHeight="1">
+    <row r="21" spans="1:12" ht="16.5" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="16.5" customHeight="1">
+    <row r="22" spans="1:12" ht="16.5" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="J22" s="1" t="b">
+      <c r="K22" s="1" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="L22" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="16.5" customHeight="1">
+    <row r="23" spans="1:12" ht="16.5" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="16.5" customHeight="1">
+    <row r="24" spans="1:12" ht="16.5" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="C24" s="2"/>
+      <c r="L24" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="16.5" customHeight="1">
+    <row r="25" spans="1:12" ht="16.5" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="16.5" customHeight="1">
+    <row r="26" spans="1:12" ht="16.5" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="16.5" customHeight="1">
+    <row r="27" spans="1:12" ht="16.5" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="L27" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="16.5" customHeight="1">
+    <row r="28" spans="1:12" ht="16.5" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="16.5" customHeight="1">
+    <row r="29" spans="1:12" ht="16.5" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="16.5" customHeight="1">
+    <row r="30" spans="1:12" ht="16.5" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="16.5" customHeight="1">
+    <row r="31" spans="1:12" ht="16.5" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="16.5" customHeight="1">
+    <row r="32" spans="1:12" ht="16.5" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="16.5" customHeight="1">
+    <row r="33" spans="1:16" ht="16.5" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="16.5" customHeight="1">
+    <row r="34" spans="1:16" ht="16.5" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="16.5" customHeight="1">
+    <row r="35" spans="1:16" ht="16.5" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="16.5" customHeight="1">
+    <row r="36" spans="1:16" ht="16.5" customHeight="1">
       <c r="A36" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="16.5" customHeight="1">
+    <row r="37" spans="1:16" ht="16.5" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="16.5" customHeight="1">
+    <row r="38" spans="1:16" ht="16.5" customHeight="1">
       <c r="A38" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="16.5" customHeight="1">
+    <row r="39" spans="1:16" ht="16.5" customHeight="1">
       <c r="A39" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="16.5" customHeight="1">
+    <row r="40" spans="1:16" ht="16.5" customHeight="1">
       <c r="A40" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="O40" s="1" t="s">
+      <c r="P40" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="16.5" customHeight="1">
+    <row r="41" spans="1:16" ht="16.5" customHeight="1">
       <c r="A41" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="16.5" customHeight="1">
+    <row r="42" spans="1:16" ht="16.5" customHeight="1">
       <c r="A42" s="1" t="s">
         <v>112</v>
       </c>
@@ -1555,18 +1566,18 @@
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="16.5" customHeight="1">
+    <row r="43" spans="1:16" ht="16.5" customHeight="1">
       <c r="A43" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="16.5" customHeight="1">
+    <row r="44" spans="1:16" ht="16.5" customHeight="1">
       <c r="A44" s="1" t="s">
         <v>115</v>
       </c>
@@ -1574,18 +1585,18 @@
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="16.5" customHeight="1">
+    <row r="45" spans="1:16" ht="16.5" customHeight="1">
       <c r="A45" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="16.5" customHeight="1">
+    <row r="46" spans="1:16" ht="16.5" customHeight="1">
       <c r="A46" s="1" t="s">
         <v>118</v>
       </c>
@@ -1593,18 +1604,18 @@
         <v>118</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="16.5" customHeight="1">
+    <row r="47" spans="1:16" ht="16.5" customHeight="1">
       <c r="A47" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="16.5" customHeight="1">
+    <row r="48" spans="1:16" ht="16.5" customHeight="1">
       <c r="A48" s="1" t="s">
         <v>121</v>
       </c>
@@ -1612,18 +1623,18 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:25" ht="16.5" customHeight="1">
+    <row r="49" spans="1:26" ht="16.5" customHeight="1">
       <c r="A49" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:25" s="1" customFormat="1" ht="16.5" customHeight="1">
+    <row r="50" spans="1:26" s="1" customFormat="1" ht="16.5" customHeight="1">
       <c r="A50" s="1" t="s">
         <v>169</v>
       </c>
@@ -1631,18 +1642,18 @@
         <v>170</v>
       </c>
     </row>
-    <row r="51" spans="1:25" s="1" customFormat="1" ht="16.5" customHeight="1">
+    <row r="51" spans="1:26" s="1" customFormat="1" ht="16.5" customHeight="1">
       <c r="A51" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="52" spans="1:25" ht="16.5" customHeight="1">
+    <row r="52" spans="1:26" ht="16.5" customHeight="1">
       <c r="A52" s="1" t="s">
         <v>124</v>
       </c>
@@ -1650,18 +1661,18 @@
         <v>124</v>
       </c>
     </row>
-    <row r="53" spans="1:25" ht="16.5" customHeight="1">
+    <row r="53" spans="1:26" ht="16.5" customHeight="1">
       <c r="A53" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="54" spans="1:25" ht="16.5" customHeight="1">
+    <row r="54" spans="1:26" ht="16.5" customHeight="1">
       <c r="A54" s="1" t="s">
         <v>127</v>
       </c>
@@ -1669,29 +1680,29 @@
         <v>127</v>
       </c>
     </row>
-    <row r="55" spans="1:25" ht="16.5" customHeight="1">
+    <row r="55" spans="1:26" ht="16.5" customHeight="1">
       <c r="A55" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="56" spans="1:25" ht="16.5" customHeight="1">
+    <row r="56" spans="1:26" ht="16.5" customHeight="1">
       <c r="A56" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="E56" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="57" spans="1:25" ht="16.5" customHeight="1">
+    <row r="57" spans="1:26" ht="16.5" customHeight="1">
       <c r="A57" s="1" t="s">
         <v>25</v>
       </c>
@@ -1699,11 +1710,11 @@
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="58" spans="1:25" ht="16.5" customHeight="1">
+    <row r="58" spans="1:26" ht="16.5" customHeight="1">
       <c r="A58" s="1" t="s">
         <v>73</v>
       </c>
@@ -1711,23 +1722,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:25">
+    <row r="59" spans="1:26">
       <c r="A59" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="K59" s="1" t="s">
+      <c r="L59" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="X59" s="1" t="s">
+      <c r="Y59" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="Y59" s="1" t="s">
+      <c r="Z59" s="1" t="s">
         <v>165</v>
       </c>
     </row>

</xml_diff>